<commit_message>
Changed logic to checkout on platform
</commit_message>
<xml_diff>
--- a/user_creds/user_credentials.xlsx
+++ b/user_creds/user_credentials.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\shoptype-automation\user_creds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\shoptype\user_creds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EDCFB6-AC31-4E73-87A5-3A46B203F68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69B01F6-AEAF-43C6-936E-FAADA4FED0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="4" r:id="rId1"/>
     <sheet name="Vendor 1" sheetId="1" r:id="rId2"/>
     <sheet name="Vendor 2" sheetId="5" r:id="rId3"/>
     <sheet name="Coseller" sheetId="2" r:id="rId4"/>
-    <sheet name="Specific Product" sheetId="6" r:id="rId5"/>
-    <sheet name="List of Products" sheetId="7" r:id="rId6"/>
+    <sheet name="List of Products" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -36,9 +35,6 @@
     <t>#Kiran1234</t>
   </si>
   <si>
-    <t>sheroesapi1@mailinator.com</t>
-  </si>
-  <si>
     <t>sheroesapi2@mailinator.com</t>
   </si>
   <si>
@@ -51,18 +47,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>product_url_1</t>
-  </si>
-  <si>
-    <t>product_url_2</t>
-  </si>
-  <si>
-    <t>https://beta.shoptype.com/product/30a976e1-aaee-d87f-b687-22a9c354d954?tid=pv_7007d6ef-b6fd-c798-5f56-6636fe8bc99e&amp;utm_medium=copy</t>
-  </si>
-  <si>
-    <t>https://beta.shoptype.com/product/c4ad560c-f27a-ed75-b7e3-a4b96c4c404d?tid=pv_cb4f0617-da21-767b-8b8d-fcc47fb6d65e&amp;utm_medium=copy</t>
-  </si>
-  <si>
     <t>product_urls</t>
   </si>
   <si>
@@ -82,6 +66,9 @@
   </si>
   <si>
     <t>https://beta.shoptype.com/product/c36929c3-56f3-97b2-28f6-ab4fa762fbfe?tid=pv_10184d36-c2f9-fcea-33d6-961e04cedd12&amp;utm_medium=copy</t>
+  </si>
+  <si>
+    <t>newnetwork1@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -465,7 +452,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,7 +471,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -492,7 +479,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -508,7 +495,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,7 +514,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -565,7 +552,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -604,7 +591,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -619,43 +606,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC62E89F-987A-4A43-B8E0-D5C2CBC8A9D0}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="44.21875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="44.77734375" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF56937C-B27B-4EBA-9227-A85D89C30090}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -671,37 +621,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test cases related to notification
</commit_message>
<xml_diff>
--- a/user_creds/user_credentials.xlsx
+++ b/user_creds/user_credentials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\shoptype\user_creds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69B01F6-AEAF-43C6-936E-FAADA4FED0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB67F1C8-8141-41E3-8AD9-EA05282990D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="4" r:id="rId1"/>
@@ -35,9 +35,6 @@
     <t>#Kiran1234</t>
   </si>
   <si>
-    <t>sheroesapi2@mailinator.com</t>
-  </si>
-  <si>
     <t>sheroesapi3@mailinator.com</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>newnetwork1@mailinator.com</t>
+  </si>
+  <si>
+    <t>notification2@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -479,7 +479,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,7 +514,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -609,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF56937C-B27B-4EBA-9227-A85D89C30090}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -621,37 +621,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed creds for usser accounts
</commit_message>
<xml_diff>
--- a/user_creds/user_credentials.xlsx
+++ b/user_creds/user_credentials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\shoptype\user_creds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB67F1C8-8141-41E3-8AD9-EA05282990D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AED76F-E4CF-48F8-AA7D-2D380D5FA7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -35,40 +35,31 @@
     <t>#Kiran1234</t>
   </si>
   <si>
-    <t>sheroesapi3@mailinator.com</t>
-  </si>
-  <si>
-    <t>sheroesapi10@mailinator.com</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>product_urls</t>
   </si>
   <si>
-    <t>https://beta.shoptype.com/product/565a25fe-932d-ff1f-632c-f9c268b41ae8?tid=pv_bd566db1-2973-ca4d-af52-7537dfd11e2f&amp;utm_medium=copy</t>
-  </si>
-  <si>
-    <t>https://beta.shoptype.com/product/fc693d0c-6326-c538-f09d-d6a4d9e2bd4e?tid=pv_63659986-17cd-63fd-f5cd-b3bfd3ce52ec&amp;utm_medium=copy</t>
-  </si>
-  <si>
-    <t>https://beta.shoptype.com/product/b83acea3-ee27-48d0-eaa7-59041a90a96c?tid=pv_df2c96f7-2ddd-30f0-5274-a560a6d190c9&amp;utm_medium=copy</t>
-  </si>
-  <si>
-    <t>https://beta.shoptype.com/product/23d9ac0d-d7b9-89ce-7ff6-1e0caa452491?tid=pv_f3b5f66f-3391-61f7-56e9-a1bb70e82227&amp;utm_medium=copy</t>
-  </si>
-  <si>
-    <t>https://beta.shoptype.com/product/59994ad2-6b1d-3724-5089-2e687c705552?tid=pv_867791cf-a52f-252f-c421-943e4a72bff3&amp;utm_medium=copy</t>
-  </si>
-  <si>
-    <t>https://beta.shoptype.com/product/c36929c3-56f3-97b2-28f6-ab4fa762fbfe?tid=pv_10184d36-c2f9-fcea-33d6-961e04cedd12&amp;utm_medium=copy</t>
-  </si>
-  <si>
-    <t>newnetwork1@mailinator.com</t>
-  </si>
-  <si>
-    <t>notification2@mailinator.com</t>
+    <t>sanitynetwork@mailinator.com</t>
+  </si>
+  <si>
+    <t>sanityvendor@mailinator.com</t>
+  </si>
+  <si>
+    <t>sanityvendor1@mailinator.com</t>
+  </si>
+  <si>
+    <t>sanitycoseller@mailinator.com</t>
+  </si>
+  <si>
+    <t>https://beta.shoptype.com/product/5af42689-ef65-295b-0193-b31cdbd47c4b?tid=pv_71832512-5344-5d1a-3dae-5e5ebfec4658&amp;utm_medium=copy</t>
+  </si>
+  <si>
+    <t>https://beta.shoptype.com/product/e9f70e52-589f-d095-b979-486d6fc5366d?tid=pv_295ecb00-15bc-0369-fc29-2731103beb41&amp;utm_medium=copy</t>
+  </si>
+  <si>
+    <t>https://beta.shoptype.com/product/df98c477-7bc9-be70-2750-17dae5f0d360?tid=pv_7a6e2d1d-f6cd-4d70-73ec-e27ec59047de&amp;utm_medium=copy</t>
   </si>
 </sst>
 </file>
@@ -451,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F041DCF-9E43-4351-838F-17AFE4DF53EF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,7 +462,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -479,12 +470,12 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7608B465-775F-42E2-BDE0-5DB3FD8D1A4E}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CD878AD0-4B8F-443E-A002-9EA327CDB490}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -494,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -514,7 +505,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -522,7 +513,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{27C8DF0B-C7AE-4B23-B34B-9233FE52C01B}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{524972C2-FC01-40D7-A223-F04260E932B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -552,7 +543,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -560,7 +551,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{9EE16DBD-9AED-43E5-9F66-D9FCAE932301}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1D78AE7A-9679-4D5B-9236-7B90F81B72FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -591,7 +582,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -599,7 +590,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{B275370D-DF89-49DF-AE7D-D227D35084D8}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EEE45F14-E2B0-4B7C-8ED6-EB109D663F31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -610,7 +601,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,38 +612,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added logic to handle authorize payments
</commit_message>
<xml_diff>
--- a/user_creds/user_credentials.xlsx
+++ b/user_creds/user_credentials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\shoptype\user_creds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AED76F-E4CF-48F8-AA7D-2D380D5FA7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D48AA4-E1B7-4E03-AC9F-7F23F1D0564A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="4" r:id="rId1"/>
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F041DCF-9E43-4351-838F-17AFE4DF53EF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF56937C-B27B-4EBA-9227-A85D89C30090}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Handled stripe kyc error and changed waits while importing products
</commit_message>
<xml_diff>
--- a/user_creds/user_credentials.xlsx
+++ b/user_creds/user_credentials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\shoptype\user_creds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D48AA4-E1B7-4E03-AC9F-7F23F1D0564A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E684639D-E12D-469F-8B62-AB262B801771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,18 +41,6 @@
     <t>product_urls</t>
   </si>
   <si>
-    <t>sanitynetwork@mailinator.com</t>
-  </si>
-  <si>
-    <t>sanityvendor@mailinator.com</t>
-  </si>
-  <si>
-    <t>sanityvendor1@mailinator.com</t>
-  </si>
-  <si>
-    <t>sanitycoseller@mailinator.com</t>
-  </si>
-  <si>
     <t>https://beta.shoptype.com/product/5af42689-ef65-295b-0193-b31cdbd47c4b?tid=pv_71832512-5344-5d1a-3dae-5e5ebfec4658&amp;utm_medium=copy</t>
   </si>
   <si>
@@ -60,6 +48,18 @@
   </si>
   <si>
     <t>https://beta.shoptype.com/product/df98c477-7bc9-be70-2750-17dae5f0d360?tid=pv_7a6e2d1d-f6cd-4d70-73ec-e27ec59047de&amp;utm_medium=copy</t>
+  </si>
+  <si>
+    <t>networkautomation1@mailinator.com</t>
+  </si>
+  <si>
+    <t>vendorautomation@mailinator.com</t>
+  </si>
+  <si>
+    <t>vendorautomation2@mailinator.com</t>
+  </si>
+  <si>
+    <t>cosellerautomation@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -475,9 +475,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CD878AD0-4B8F-443E-A002-9EA327CDB490}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{24F12C54-E62C-4E74-9A4D-95811D23E155}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -505,7 +506,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -513,9 +514,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{524972C2-FC01-40D7-A223-F04260E932B2}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4C7C869B-5780-4393-ACD7-A2F7DCBCE71C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -543,7 +545,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -551,7 +553,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{1D78AE7A-9679-4D5B-9236-7B90F81B72FE}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D15A60E6-474A-498F-9E83-79A5C38FB1BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -582,7 +584,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -590,7 +592,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{EEE45F14-E2B0-4B7C-8ED6-EB109D663F31}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{23B8E841-E932-493E-9376-192CB7EC1920}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -601,7 +603,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,17 +619,17 @@
     </row>
     <row r="2" spans="1:1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>